<commit_message>
Add change 18 APril
</commit_message>
<xml_diff>
--- a/docs/assets/data/credentials.xlsx
+++ b/docs/assets/data/credentials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\monal\OneDrive\Desktop\A2N.AI-II\Build-demo\A2N-AI-Demo\docs\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{145A95AE-C244-4EF2-A287-62E8ED31A4D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2AF09B3-8291-4859-AE56-A50DFDF47D22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>username</t>
   </si>
@@ -37,9 +37,6 @@
   </si>
   <si>
     <t>a2n@gmail.com</t>
-  </si>
-  <si>
-    <t>arn@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -400,16 +397,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="16.7265625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
@@ -432,14 +426,6 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
         <v>2</v>
       </c>
     </row>
@@ -447,10 +433,9 @@
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="A3" r:id="rId2" xr:uid="{60B9BDE7-6614-4ED2-9F86-F531C305DAC9}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{B4C77A5E-C8AF-4D48-9A1E-A8C318ABB395}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>